<commit_message>
Guía Didáctica MA_07_07_CO y MA_07_08_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion08/ESCALETA_MA_07_08_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion08/ESCALETA_MA_07_08_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Copia\JOHANNA\Documents\Documents\Matematicas\fuentes\contenidos\grado07\guion08\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -1141,6 +1146,21 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1199,21 +1219,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1276,7 +1281,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1311,7 +1316,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1522,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1553,94 +1558,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="96" t="s">
         <v>172</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="98" t="s">
         <v>173</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="102" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="I1" s="104" t="s">
         <v>175</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="85" t="s">
+      <c r="K1" s="90" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="84" t="s">
+      <c r="L1" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="88" t="s">
+      <c r="M1" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="88"/>
-      <c r="O1" s="81" t="s">
+      <c r="N1" s="93"/>
+      <c r="O1" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="101" t="s">
+      <c r="P1" s="81" t="s">
         <v>176</v>
       </c>
-      <c r="Q1" s="102" t="s">
+      <c r="Q1" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="R1" s="105" t="s">
+      <c r="R1" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="S1" s="104" t="s">
+      <c r="S1" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="103" t="s">
+      <c r="T1" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="U1" s="102" t="s">
+      <c r="U1" s="82" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="84"/>
+      <c r="A2" s="88"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="89"/>
       <c r="M2" s="34" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="O2" s="81"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="105"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="102"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="82"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
@@ -3327,12 +3332,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -3347,6 +3346,12 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M31">

</xml_diff>